<commit_message>
Victory reports and dashboard work
</commit_message>
<xml_diff>
--- a/Documentation/Account upload.xlsx
+++ b/Documentation/Account upload.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10913"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10323"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/darryllrobinson/Documents/projects/ciab/documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/darryllrobinson/Documents/projects/thesystem/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1A6A727-9EE1-0540-9F47-8BC3F8AD721A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D26BA99A-E5E1-6F41-A9F6-0B66CBFC9B3D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28380" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28380" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Account" sheetId="11" r:id="rId1"/>
@@ -453,7 +453,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy/mm/dd;@"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -463,12 +463,6 @@
     </font>
     <font>
       <sz val="10"/>
-      <name val="Abadi Extra Light"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color theme="1"/>
       <name val="Abadi Extra Light"/>
       <family val="2"/>
     </font>
@@ -499,7 +493,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -516,10 +510,6 @@
     <xf numFmtId="4" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="4" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="4" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -809,9 +799,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1AC8A94F-0D88-45B1-B60B-5C961E12494A}">
   <dimension ref="A1:T51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="S5" sqref="S5"/>
+      <selection pane="bottomLeft" activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -825,17 +815,18 @@
     <col min="7" max="7" width="8.83203125" style="5" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="10.5" style="5" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="12.1640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="10" max="12" width="6.6640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="13" max="15" width="7.83203125" style="5" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="11.5" style="8" bestFit="1" customWidth="1"/>
+    <col min="10" max="12" width="8.83203125" style="5" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="7.83203125" style="5" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="8.83203125" style="5" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11.5" style="6" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="13.1640625" style="1" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="4" style="1" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="11.5" style="10" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="11.5" style="8" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="25.5" style="1" bestFit="1" customWidth="1"/>
     <col min="21" max="16384" width="8.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="12" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:20" ht="13" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>120</v>
       </c>
@@ -890,14 +881,14 @@
       <c r="R1" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="S1" s="10" t="s">
+      <c r="S1" s="8" t="s">
         <v>110</v>
       </c>
-      <c r="T1" s="9" t="s">
+      <c r="T1" s="7" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="2" spans="1:20" ht="12" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:20" ht="13" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>121</v>
       </c>
@@ -913,22 +904,54 @@
       <c r="F2" s="1">
         <v>7</v>
       </c>
-      <c r="I2" s="6"/>
-      <c r="P2" s="5"/>
+      <c r="H2" s="5">
+        <v>0</v>
+      </c>
+      <c r="I2" s="5">
+        <f>P2*2</f>
+        <v>0</v>
+      </c>
+      <c r="J2" s="5">
+        <f>I2*0.8</f>
+        <v>0</v>
+      </c>
+      <c r="K2" s="5">
+        <f>I2*1.1</f>
+        <v>0</v>
+      </c>
+      <c r="L2" s="5">
+        <f>I2*1.4</f>
+        <v>0</v>
+      </c>
+      <c r="M2" s="5">
+        <f>I2*1.7</f>
+        <v>0</v>
+      </c>
+      <c r="N2" s="5">
+        <f>I2*0.1</f>
+        <v>0</v>
+      </c>
+      <c r="O2" s="5">
+        <f>I2*0.05</f>
+        <v>0</v>
+      </c>
+      <c r="P2" s="5">
+        <v>0</v>
+      </c>
       <c r="Q2" s="1" t="s">
         <v>98</v>
       </c>
       <c r="R2" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="S2" s="10">
+      <c r="S2" s="8">
         <v>44089</v>
       </c>
       <c r="T2" s="1" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="3" spans="1:20" ht="12" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:20" ht="13" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>121</v>
       </c>
@@ -944,21 +967,54 @@
       <c r="F3" s="1">
         <v>7</v>
       </c>
-      <c r="P3" s="5"/>
+      <c r="H3" s="5">
+        <v>0</v>
+      </c>
+      <c r="I3" s="5">
+        <f>P3*0.5</f>
+        <v>0</v>
+      </c>
+      <c r="J3" s="5">
+        <f>I3*0.3</f>
+        <v>0</v>
+      </c>
+      <c r="K3" s="5">
+        <f>I3*1.2</f>
+        <v>0</v>
+      </c>
+      <c r="L3" s="5">
+        <f>I3*1.5</f>
+        <v>0</v>
+      </c>
+      <c r="M3" s="5">
+        <f>I3*1.9</f>
+        <v>0</v>
+      </c>
+      <c r="N3" s="5">
+        <f>I3*0.2</f>
+        <v>0</v>
+      </c>
+      <c r="O3" s="5">
+        <f>I3*1.3</f>
+        <v>0</v>
+      </c>
+      <c r="P3" s="5">
+        <v>0</v>
+      </c>
       <c r="Q3" s="1" t="s">
         <v>98</v>
       </c>
       <c r="R3" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="S3" s="10">
+      <c r="S3" s="8">
         <v>44089</v>
       </c>
       <c r="T3" s="1" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="4" spans="1:20" ht="12" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:20" ht="13" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>121</v>
       </c>
@@ -974,6 +1030,34 @@
       <c r="H4" s="5">
         <v>16915.78</v>
       </c>
+      <c r="I4" s="5">
+        <f>P4</f>
+        <v>16915.78</v>
+      </c>
+      <c r="J4" s="5">
+        <f>I4*0</f>
+        <v>0</v>
+      </c>
+      <c r="K4" s="5">
+        <f>I4*1.3</f>
+        <v>21990.513999999999</v>
+      </c>
+      <c r="L4" s="5">
+        <f>I4*1.6</f>
+        <v>27065.248</v>
+      </c>
+      <c r="M4" s="5">
+        <f>I4*0.2</f>
+        <v>3383.1559999999999</v>
+      </c>
+      <c r="N4" s="5">
+        <f>I4*0.5</f>
+        <v>8457.89</v>
+      </c>
+      <c r="O4" s="5">
+        <f>I4*1.76</f>
+        <v>29771.772799999999</v>
+      </c>
       <c r="P4" s="5">
         <v>16915.78</v>
       </c>
@@ -981,7 +1065,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="5" spans="1:20" ht="12" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:20" ht="13" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>121</v>
       </c>
@@ -1000,10 +1084,34 @@
       <c r="H5" s="5">
         <v>29934.84</v>
       </c>
-      <c r="I5" s="6"/>
-      <c r="M5" s="7"/>
-      <c r="N5" s="7"/>
-      <c r="O5" s="7"/>
+      <c r="I5" s="5">
+        <f t="shared" ref="I5:I51" si="0">P5*2</f>
+        <v>59869.68</v>
+      </c>
+      <c r="J5" s="5">
+        <f t="shared" ref="J5" si="1">I5*0.8</f>
+        <v>47895.744000000006</v>
+      </c>
+      <c r="K5" s="5">
+        <f t="shared" ref="K5:K51" si="2">I5*1.1</f>
+        <v>65856.648000000001</v>
+      </c>
+      <c r="L5" s="5">
+        <f t="shared" ref="L5:L51" si="3">I5*1.4</f>
+        <v>83817.551999999996</v>
+      </c>
+      <c r="M5" s="5">
+        <f t="shared" ref="M5:M51" si="4">I5*1.7</f>
+        <v>101778.45599999999</v>
+      </c>
+      <c r="N5" s="5">
+        <f t="shared" ref="N5:N51" si="5">I5*0.1</f>
+        <v>5986.9680000000008</v>
+      </c>
+      <c r="O5" s="5">
+        <f t="shared" ref="O5:O51" si="6">I5*0.05</f>
+        <v>2993.4840000000004</v>
+      </c>
       <c r="P5" s="5">
         <v>29934.84</v>
       </c>
@@ -1017,7 +1125,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="6" spans="1:20" ht="12" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:20" ht="13" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>121</v>
       </c>
@@ -1036,6 +1144,34 @@
       <c r="H6" s="5">
         <v>34658.080000000002</v>
       </c>
+      <c r="I6" s="5">
+        <f t="shared" ref="I6:I51" si="7">P6*0.5</f>
+        <v>17329.04</v>
+      </c>
+      <c r="J6" s="5">
+        <f t="shared" ref="J6" si="8">I6*0.3</f>
+        <v>5198.7120000000004</v>
+      </c>
+      <c r="K6" s="5">
+        <f t="shared" ref="K6:K51" si="9">I6*1.2</f>
+        <v>20794.848000000002</v>
+      </c>
+      <c r="L6" s="5">
+        <f t="shared" ref="L6:L51" si="10">I6*1.5</f>
+        <v>25993.56</v>
+      </c>
+      <c r="M6" s="5">
+        <f t="shared" ref="M6:M51" si="11">I6*1.9</f>
+        <v>32925.175999999999</v>
+      </c>
+      <c r="N6" s="5">
+        <f t="shared" ref="N6:N51" si="12">I6*0.2</f>
+        <v>3465.8080000000004</v>
+      </c>
+      <c r="O6" s="5">
+        <f t="shared" ref="O6:O51" si="13">I6*1.3</f>
+        <v>22527.752</v>
+      </c>
       <c r="P6" s="5">
         <v>34658.080000000002</v>
       </c>
@@ -1045,14 +1181,14 @@
       <c r="R6" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="S6" s="10">
+      <c r="S6" s="8">
         <v>43038</v>
       </c>
       <c r="T6" s="1" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="7" spans="1:20" ht="12" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:20" ht="13" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>121</v>
       </c>
@@ -1071,6 +1207,34 @@
       <c r="H7" s="5">
         <v>8889.5</v>
       </c>
+      <c r="I7" s="5">
+        <f t="shared" ref="I7:I51" si="14">P7</f>
+        <v>8889.5</v>
+      </c>
+      <c r="J7" s="5">
+        <f t="shared" ref="J7" si="15">I7*0</f>
+        <v>0</v>
+      </c>
+      <c r="K7" s="5">
+        <f t="shared" ref="K7:K51" si="16">I7*1.3</f>
+        <v>11556.35</v>
+      </c>
+      <c r="L7" s="5">
+        <f t="shared" ref="L7:L51" si="17">I7*1.6</f>
+        <v>14223.2</v>
+      </c>
+      <c r="M7" s="5">
+        <f t="shared" ref="M7:M51" si="18">I7*0.2</f>
+        <v>1777.9</v>
+      </c>
+      <c r="N7" s="5">
+        <f t="shared" ref="N7:N51" si="19">I7*0.5</f>
+        <v>4444.75</v>
+      </c>
+      <c r="O7" s="5">
+        <f t="shared" ref="O7:O51" si="20">I7*1.76</f>
+        <v>15645.52</v>
+      </c>
       <c r="P7" s="5">
         <v>8889.5</v>
       </c>
@@ -1084,7 +1248,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="8" spans="1:20" ht="12" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:20" ht="13" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>121</v>
       </c>
@@ -1104,6 +1268,34 @@
       <c r="H8" s="5">
         <v>5000.01</v>
       </c>
+      <c r="I8" s="5">
+        <f t="shared" ref="I8:I51" si="21">P8*2</f>
+        <v>10000.02</v>
+      </c>
+      <c r="J8" s="5">
+        <f t="shared" ref="J8" si="22">I8*0.8</f>
+        <v>8000.0160000000005</v>
+      </c>
+      <c r="K8" s="5">
+        <f t="shared" ref="K8:K51" si="23">I8*1.1</f>
+        <v>11000.022000000001</v>
+      </c>
+      <c r="L8" s="5">
+        <f t="shared" ref="L8:L51" si="24">I8*1.4</f>
+        <v>14000.028</v>
+      </c>
+      <c r="M8" s="5">
+        <f t="shared" ref="M8:M51" si="25">I8*1.7</f>
+        <v>17000.034</v>
+      </c>
+      <c r="N8" s="5">
+        <f t="shared" ref="N8:N51" si="26">I8*0.1</f>
+        <v>1000.0020000000001</v>
+      </c>
+      <c r="O8" s="5">
+        <f t="shared" ref="O8:O51" si="27">I8*0.05</f>
+        <v>500.00100000000003</v>
+      </c>
       <c r="P8" s="5">
         <v>5000.01</v>
       </c>
@@ -1117,7 +1309,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="9" spans="1:20" ht="12" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:20" ht="13" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>121</v>
       </c>
@@ -1136,6 +1328,34 @@
       <c r="H9" s="5">
         <v>23913.85</v>
       </c>
+      <c r="I9" s="5">
+        <f t="shared" ref="I9:I51" si="28">P9*0.5</f>
+        <v>11956.924999999999</v>
+      </c>
+      <c r="J9" s="5">
+        <f t="shared" ref="J9" si="29">I9*0.3</f>
+        <v>3587.0774999999999</v>
+      </c>
+      <c r="K9" s="5">
+        <f t="shared" ref="K9:K51" si="30">I9*1.2</f>
+        <v>14348.31</v>
+      </c>
+      <c r="L9" s="5">
+        <f t="shared" ref="L9:L51" si="31">I9*1.5</f>
+        <v>17935.387499999997</v>
+      </c>
+      <c r="M9" s="5">
+        <f t="shared" ref="M9:M51" si="32">I9*1.9</f>
+        <v>22718.157499999998</v>
+      </c>
+      <c r="N9" s="5">
+        <f t="shared" ref="N9:N51" si="33">I9*0.2</f>
+        <v>2391.3849999999998</v>
+      </c>
+      <c r="O9" s="5">
+        <f t="shared" ref="O9:O51" si="34">I9*1.3</f>
+        <v>15544.002499999999</v>
+      </c>
       <c r="P9" s="5">
         <v>23913.85</v>
       </c>
@@ -1145,14 +1365,14 @@
       <c r="R9" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="S9" s="10">
+      <c r="S9" s="8">
         <v>42951</v>
       </c>
       <c r="T9" s="1" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="10" spans="1:20" ht="12" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:20" ht="13" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>121</v>
       </c>
@@ -1171,7 +1391,34 @@
       <c r="H10" s="5">
         <v>14947.7</v>
       </c>
-      <c r="I10" s="6"/>
+      <c r="I10" s="5">
+        <f t="shared" ref="I10:I51" si="35">P10</f>
+        <v>14947.7</v>
+      </c>
+      <c r="J10" s="5">
+        <f t="shared" ref="J10" si="36">I10*0</f>
+        <v>0</v>
+      </c>
+      <c r="K10" s="5">
+        <f t="shared" ref="K10:K51" si="37">I10*1.3</f>
+        <v>19432.010000000002</v>
+      </c>
+      <c r="L10" s="5">
+        <f t="shared" ref="L10:L51" si="38">I10*1.6</f>
+        <v>23916.320000000003</v>
+      </c>
+      <c r="M10" s="5">
+        <f t="shared" ref="M10:M51" si="39">I10*0.2</f>
+        <v>2989.5400000000004</v>
+      </c>
+      <c r="N10" s="5">
+        <f t="shared" ref="N10:N51" si="40">I10*0.5</f>
+        <v>7473.85</v>
+      </c>
+      <c r="O10" s="5">
+        <f t="shared" ref="O10:O51" si="41">I10*1.76</f>
+        <v>26307.952000000001</v>
+      </c>
       <c r="P10" s="5">
         <v>14947.7</v>
       </c>
@@ -1185,7 +1432,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="11" spans="1:20" ht="12" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:20" ht="13" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>121</v>
       </c>
@@ -1204,6 +1451,34 @@
       <c r="H11" s="5">
         <v>8746.2800000000007</v>
       </c>
+      <c r="I11" s="5">
+        <f t="shared" ref="I11:I51" si="42">P11*2</f>
+        <v>17492.560000000001</v>
+      </c>
+      <c r="J11" s="5">
+        <f t="shared" ref="J11" si="43">I11*0.8</f>
+        <v>13994.048000000003</v>
+      </c>
+      <c r="K11" s="5">
+        <f t="shared" ref="K11:K51" si="44">I11*1.1</f>
+        <v>19241.816000000003</v>
+      </c>
+      <c r="L11" s="5">
+        <f t="shared" ref="L11:L51" si="45">I11*1.4</f>
+        <v>24489.583999999999</v>
+      </c>
+      <c r="M11" s="5">
+        <f t="shared" ref="M11:M51" si="46">I11*1.7</f>
+        <v>29737.352000000003</v>
+      </c>
+      <c r="N11" s="5">
+        <f t="shared" ref="N11:N51" si="47">I11*0.1</f>
+        <v>1749.2560000000003</v>
+      </c>
+      <c r="O11" s="5">
+        <f t="shared" ref="O11:O51" si="48">I11*0.05</f>
+        <v>874.62800000000016</v>
+      </c>
       <c r="P11" s="5">
         <v>8746.2800000000007</v>
       </c>
@@ -1213,14 +1488,14 @@
       <c r="R11" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="S11" s="10">
+      <c r="S11" s="8">
         <v>42859</v>
       </c>
       <c r="T11" s="1" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="12" spans="1:20" ht="12" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:20" ht="13" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>121</v>
       </c>
@@ -1236,6 +1511,34 @@
       <c r="H12" s="5">
         <v>87175.63</v>
       </c>
+      <c r="I12" s="5">
+        <f t="shared" ref="I12:I51" si="49">P12*0.5</f>
+        <v>43587.815000000002</v>
+      </c>
+      <c r="J12" s="5">
+        <f t="shared" ref="J12" si="50">I12*0.3</f>
+        <v>13076.344500000001</v>
+      </c>
+      <c r="K12" s="5">
+        <f t="shared" ref="K12:K51" si="51">I12*1.2</f>
+        <v>52305.378000000004</v>
+      </c>
+      <c r="L12" s="5">
+        <f t="shared" ref="L12:L51" si="52">I12*1.5</f>
+        <v>65381.722500000003</v>
+      </c>
+      <c r="M12" s="5">
+        <f t="shared" ref="M12:M51" si="53">I12*1.9</f>
+        <v>82816.848500000007</v>
+      </c>
+      <c r="N12" s="5">
+        <f t="shared" ref="N12:N51" si="54">I12*0.2</f>
+        <v>8717.5630000000001</v>
+      </c>
+      <c r="O12" s="5">
+        <f t="shared" ref="O12:O51" si="55">I12*1.3</f>
+        <v>56664.159500000002</v>
+      </c>
       <c r="P12" s="5">
         <v>87175.63</v>
       </c>
@@ -1243,7 +1546,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="13" spans="1:20" ht="12" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:20" ht="13" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>121</v>
       </c>
@@ -1263,6 +1566,34 @@
       <c r="H13" s="5">
         <v>5694.43</v>
       </c>
+      <c r="I13" s="5">
+        <f t="shared" ref="I13:I51" si="56">P13</f>
+        <v>5694.43</v>
+      </c>
+      <c r="J13" s="5">
+        <f t="shared" ref="J13" si="57">I13*0</f>
+        <v>0</v>
+      </c>
+      <c r="K13" s="5">
+        <f t="shared" ref="K13:K51" si="58">I13*1.3</f>
+        <v>7402.7590000000009</v>
+      </c>
+      <c r="L13" s="5">
+        <f t="shared" ref="L13:L51" si="59">I13*1.6</f>
+        <v>9111.0880000000016</v>
+      </c>
+      <c r="M13" s="5">
+        <f t="shared" ref="M13:M51" si="60">I13*0.2</f>
+        <v>1138.8860000000002</v>
+      </c>
+      <c r="N13" s="5">
+        <f t="shared" ref="N13:N51" si="61">I13*0.5</f>
+        <v>2847.2150000000001</v>
+      </c>
+      <c r="O13" s="5">
+        <f t="shared" ref="O13:O51" si="62">I13*1.76</f>
+        <v>10022.1968</v>
+      </c>
       <c r="P13" s="5">
         <v>5694.43</v>
       </c>
@@ -1276,7 +1607,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="14" spans="1:20" ht="12" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:20" ht="13" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>121</v>
       </c>
@@ -1295,7 +1626,34 @@
       <c r="H14" s="5">
         <v>5100</v>
       </c>
-      <c r="I14" s="6"/>
+      <c r="I14" s="5">
+        <f t="shared" ref="I14:I51" si="63">P14*2</f>
+        <v>10200</v>
+      </c>
+      <c r="J14" s="5">
+        <f t="shared" ref="J14" si="64">I14*0.8</f>
+        <v>8160</v>
+      </c>
+      <c r="K14" s="5">
+        <f t="shared" ref="K14:K51" si="65">I14*1.1</f>
+        <v>11220</v>
+      </c>
+      <c r="L14" s="5">
+        <f t="shared" ref="L14:L51" si="66">I14*1.4</f>
+        <v>14280</v>
+      </c>
+      <c r="M14" s="5">
+        <f t="shared" ref="M14:M51" si="67">I14*1.7</f>
+        <v>17340</v>
+      </c>
+      <c r="N14" s="5">
+        <f t="shared" ref="N14:N51" si="68">I14*0.1</f>
+        <v>1020</v>
+      </c>
+      <c r="O14" s="5">
+        <f t="shared" ref="O14:O51" si="69">I14*0.05</f>
+        <v>510</v>
+      </c>
       <c r="P14" s="5">
         <v>5100</v>
       </c>
@@ -1309,7 +1667,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="15" spans="1:20" ht="12" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:20" ht="13" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>121</v>
       </c>
@@ -1328,7 +1686,34 @@
       <c r="H15" s="5">
         <v>7343.87</v>
       </c>
-      <c r="I15" s="6"/>
+      <c r="I15" s="5">
+        <f t="shared" ref="I15:I51" si="70">P15*0.5</f>
+        <v>3671.9349999999999</v>
+      </c>
+      <c r="J15" s="5">
+        <f t="shared" ref="J15" si="71">I15*0.3</f>
+        <v>1101.5805</v>
+      </c>
+      <c r="K15" s="5">
+        <f t="shared" ref="K15:K51" si="72">I15*1.2</f>
+        <v>4406.3220000000001</v>
+      </c>
+      <c r="L15" s="5">
+        <f t="shared" ref="L15:L51" si="73">I15*1.5</f>
+        <v>5507.9025000000001</v>
+      </c>
+      <c r="M15" s="5">
+        <f t="shared" ref="M15:M51" si="74">I15*1.9</f>
+        <v>6976.6764999999996</v>
+      </c>
+      <c r="N15" s="5">
+        <f t="shared" ref="N15:N51" si="75">I15*0.2</f>
+        <v>734.38700000000006</v>
+      </c>
+      <c r="O15" s="5">
+        <f t="shared" ref="O15:O51" si="76">I15*1.3</f>
+        <v>4773.5155000000004</v>
+      </c>
       <c r="P15" s="5">
         <v>7343.87</v>
       </c>
@@ -1342,7 +1727,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="16" spans="1:20" ht="12" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:20" ht="13" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>121</v>
       </c>
@@ -1361,6 +1746,34 @@
       <c r="H16" s="5">
         <v>32478.880000000001</v>
       </c>
+      <c r="I16" s="5">
+        <f t="shared" ref="I16:I51" si="77">P16</f>
+        <v>32478.880000000001</v>
+      </c>
+      <c r="J16" s="5">
+        <f t="shared" ref="J16" si="78">I16*0</f>
+        <v>0</v>
+      </c>
+      <c r="K16" s="5">
+        <f t="shared" ref="K16:K51" si="79">I16*1.3</f>
+        <v>42222.544000000002</v>
+      </c>
+      <c r="L16" s="5">
+        <f t="shared" ref="L16:L51" si="80">I16*1.6</f>
+        <v>51966.208000000006</v>
+      </c>
+      <c r="M16" s="5">
+        <f t="shared" ref="M16:M51" si="81">I16*0.2</f>
+        <v>6495.7760000000007</v>
+      </c>
+      <c r="N16" s="5">
+        <f t="shared" ref="N16:N51" si="82">I16*0.5</f>
+        <v>16239.44</v>
+      </c>
+      <c r="O16" s="5">
+        <f t="shared" ref="O16:O51" si="83">I16*1.76</f>
+        <v>57162.828800000003</v>
+      </c>
       <c r="P16" s="5">
         <v>32478.880000000001</v>
       </c>
@@ -1374,7 +1787,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="17" spans="1:20" ht="12" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:20" ht="13" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>121</v>
       </c>
@@ -1393,6 +1806,34 @@
       <c r="H17" s="5">
         <v>4325.84</v>
       </c>
+      <c r="I17" s="5">
+        <f t="shared" ref="I17:I51" si="84">P17*2</f>
+        <v>8651.68</v>
+      </c>
+      <c r="J17" s="5">
+        <f t="shared" ref="J17" si="85">I17*0.8</f>
+        <v>6921.344000000001</v>
+      </c>
+      <c r="K17" s="5">
+        <f t="shared" ref="K17:K51" si="86">I17*1.1</f>
+        <v>9516.8480000000018</v>
+      </c>
+      <c r="L17" s="5">
+        <f t="shared" ref="L17:L51" si="87">I17*1.4</f>
+        <v>12112.351999999999</v>
+      </c>
+      <c r="M17" s="5">
+        <f t="shared" ref="M17:M51" si="88">I17*1.7</f>
+        <v>14707.856</v>
+      </c>
+      <c r="N17" s="5">
+        <f t="shared" ref="N17:N51" si="89">I17*0.1</f>
+        <v>865.16800000000012</v>
+      </c>
+      <c r="O17" s="5">
+        <f t="shared" ref="O17:O51" si="90">I17*0.05</f>
+        <v>432.58400000000006</v>
+      </c>
       <c r="P17" s="5">
         <v>4325.84</v>
       </c>
@@ -1406,7 +1847,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="18" spans="1:20" ht="12" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:20" ht="13" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>121</v>
       </c>
@@ -1426,6 +1867,34 @@
       <c r="H18" s="5">
         <v>19108.419999999998</v>
       </c>
+      <c r="I18" s="5">
+        <f t="shared" ref="I18:I51" si="91">P18*0.5</f>
+        <v>9554.2099999999991</v>
+      </c>
+      <c r="J18" s="5">
+        <f t="shared" ref="J18" si="92">I18*0.3</f>
+        <v>2866.2629999999995</v>
+      </c>
+      <c r="K18" s="5">
+        <f t="shared" ref="K18:K51" si="93">I18*1.2</f>
+        <v>11465.051999999998</v>
+      </c>
+      <c r="L18" s="5">
+        <f t="shared" ref="L18:L51" si="94">I18*1.5</f>
+        <v>14331.314999999999</v>
+      </c>
+      <c r="M18" s="5">
+        <f t="shared" ref="M18:M51" si="95">I18*1.9</f>
+        <v>18152.998999999996</v>
+      </c>
+      <c r="N18" s="5">
+        <f t="shared" ref="N18:N51" si="96">I18*0.2</f>
+        <v>1910.8419999999999</v>
+      </c>
+      <c r="O18" s="5">
+        <f t="shared" ref="O18:O51" si="97">I18*1.3</f>
+        <v>12420.473</v>
+      </c>
       <c r="P18" s="5">
         <v>19108.419999999998</v>
       </c>
@@ -1439,7 +1908,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="19" spans="1:20" ht="12" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:20" ht="13" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>121</v>
       </c>
@@ -1458,9 +1927,34 @@
       <c r="H19" s="5">
         <v>12075.93</v>
       </c>
-      <c r="M19" s="7"/>
-      <c r="N19" s="7"/>
-      <c r="O19" s="7"/>
+      <c r="I19" s="5">
+        <f t="shared" ref="I19:I51" si="98">P19</f>
+        <v>12075.93</v>
+      </c>
+      <c r="J19" s="5">
+        <f t="shared" ref="J19" si="99">I19*0</f>
+        <v>0</v>
+      </c>
+      <c r="K19" s="5">
+        <f t="shared" ref="K19:K51" si="100">I19*1.3</f>
+        <v>15698.709000000001</v>
+      </c>
+      <c r="L19" s="5">
+        <f t="shared" ref="L19:L51" si="101">I19*1.6</f>
+        <v>19321.488000000001</v>
+      </c>
+      <c r="M19" s="5">
+        <f t="shared" ref="M19:M51" si="102">I19*0.2</f>
+        <v>2415.1860000000001</v>
+      </c>
+      <c r="N19" s="5">
+        <f t="shared" ref="N19:N51" si="103">I19*0.5</f>
+        <v>6037.9650000000001</v>
+      </c>
+      <c r="O19" s="5">
+        <f t="shared" ref="O19:O51" si="104">I19*1.76</f>
+        <v>21253.6368</v>
+      </c>
       <c r="P19" s="5">
         <v>12075.93</v>
       </c>
@@ -1470,14 +1964,14 @@
       <c r="R19" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="S19" s="10">
+      <c r="S19" s="8">
         <v>42851</v>
       </c>
       <c r="T19" s="1" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="20" spans="1:20" ht="12" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:20" ht="13" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>121</v>
       </c>
@@ -1497,6 +1991,34 @@
       <c r="H20" s="5">
         <v>29895.4</v>
       </c>
+      <c r="I20" s="5">
+        <f t="shared" ref="I20:I51" si="105">P20*2</f>
+        <v>59790.8</v>
+      </c>
+      <c r="J20" s="5">
+        <f t="shared" ref="J20" si="106">I20*0.8</f>
+        <v>47832.640000000007</v>
+      </c>
+      <c r="K20" s="5">
+        <f t="shared" ref="K20:K51" si="107">I20*1.1</f>
+        <v>65769.88</v>
+      </c>
+      <c r="L20" s="5">
+        <f t="shared" ref="L20:L51" si="108">I20*1.4</f>
+        <v>83707.12</v>
+      </c>
+      <c r="M20" s="5">
+        <f t="shared" ref="M20:M51" si="109">I20*1.7</f>
+        <v>101644.36</v>
+      </c>
+      <c r="N20" s="5">
+        <f t="shared" ref="N20:N51" si="110">I20*0.1</f>
+        <v>5979.0800000000008</v>
+      </c>
+      <c r="O20" s="5">
+        <f t="shared" ref="O20:O51" si="111">I20*0.05</f>
+        <v>2989.5400000000004</v>
+      </c>
       <c r="P20" s="5">
         <v>29895.4</v>
       </c>
@@ -1506,14 +2028,14 @@
       <c r="R20" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="S20" s="10">
+      <c r="S20" s="8">
         <v>42639</v>
       </c>
       <c r="T20" s="1" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="21" spans="1:20" ht="12" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:20" ht="13" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>121</v>
       </c>
@@ -1532,6 +2054,34 @@
       <c r="H21" s="5">
         <v>4810</v>
       </c>
+      <c r="I21" s="5">
+        <f t="shared" ref="I21:I51" si="112">P21*0.5</f>
+        <v>2405</v>
+      </c>
+      <c r="J21" s="5">
+        <f t="shared" ref="J21" si="113">I21*0.3</f>
+        <v>721.5</v>
+      </c>
+      <c r="K21" s="5">
+        <f t="shared" ref="K21:K51" si="114">I21*1.2</f>
+        <v>2886</v>
+      </c>
+      <c r="L21" s="5">
+        <f t="shared" ref="L21:L51" si="115">I21*1.5</f>
+        <v>3607.5</v>
+      </c>
+      <c r="M21" s="5">
+        <f t="shared" ref="M21:M51" si="116">I21*1.9</f>
+        <v>4569.5</v>
+      </c>
+      <c r="N21" s="5">
+        <f t="shared" ref="N21:N51" si="117">I21*0.2</f>
+        <v>481</v>
+      </c>
+      <c r="O21" s="5">
+        <f t="shared" ref="O21:O51" si="118">I21*1.3</f>
+        <v>3126.5</v>
+      </c>
       <c r="P21" s="5">
         <v>4810</v>
       </c>
@@ -1545,7 +2095,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="22" spans="1:20" ht="12" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:20" ht="13" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>121</v>
       </c>
@@ -1564,9 +2114,34 @@
       <c r="H22" s="5">
         <v>5495</v>
       </c>
-      <c r="M22" s="7"/>
-      <c r="N22" s="7"/>
-      <c r="O22" s="7"/>
+      <c r="I22" s="5">
+        <f t="shared" ref="I22:I51" si="119">P22</f>
+        <v>5495</v>
+      </c>
+      <c r="J22" s="5">
+        <f t="shared" ref="J22" si="120">I22*0</f>
+        <v>0</v>
+      </c>
+      <c r="K22" s="5">
+        <f t="shared" ref="K22:K51" si="121">I22*1.3</f>
+        <v>7143.5</v>
+      </c>
+      <c r="L22" s="5">
+        <f t="shared" ref="L22:L51" si="122">I22*1.6</f>
+        <v>8792</v>
+      </c>
+      <c r="M22" s="5">
+        <f t="shared" ref="M22:M51" si="123">I22*0.2</f>
+        <v>1099</v>
+      </c>
+      <c r="N22" s="5">
+        <f t="shared" ref="N22:N51" si="124">I22*0.5</f>
+        <v>2747.5</v>
+      </c>
+      <c r="O22" s="5">
+        <f t="shared" ref="O22:O51" si="125">I22*1.76</f>
+        <v>9671.2000000000007</v>
+      </c>
       <c r="P22" s="5">
         <v>5495</v>
       </c>
@@ -1576,14 +2151,14 @@
       <c r="R22" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="S22" s="10">
+      <c r="S22" s="8">
         <v>43133</v>
       </c>
       <c r="T22" s="1" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="23" spans="1:20" ht="12" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:20" ht="13" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>121</v>
       </c>
@@ -1602,6 +2177,34 @@
       <c r="H23" s="5">
         <v>5206</v>
       </c>
+      <c r="I23" s="5">
+        <f t="shared" ref="I23:I51" si="126">P23*2</f>
+        <v>10412</v>
+      </c>
+      <c r="J23" s="5">
+        <f t="shared" ref="J23" si="127">I23*0.8</f>
+        <v>8329.6</v>
+      </c>
+      <c r="K23" s="5">
+        <f t="shared" ref="K23:K51" si="128">I23*1.1</f>
+        <v>11453.2</v>
+      </c>
+      <c r="L23" s="5">
+        <f t="shared" ref="L23:L51" si="129">I23*1.4</f>
+        <v>14576.8</v>
+      </c>
+      <c r="M23" s="5">
+        <f t="shared" ref="M23:M51" si="130">I23*1.7</f>
+        <v>17700.399999999998</v>
+      </c>
+      <c r="N23" s="5">
+        <f t="shared" ref="N23:N51" si="131">I23*0.1</f>
+        <v>1041.2</v>
+      </c>
+      <c r="O23" s="5">
+        <f t="shared" ref="O23:O51" si="132">I23*0.05</f>
+        <v>520.6</v>
+      </c>
       <c r="P23" s="5">
         <v>5206</v>
       </c>
@@ -1615,7 +2218,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="24" spans="1:20" ht="12" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:20" ht="13" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>121</v>
       </c>
@@ -1634,6 +2237,34 @@
       <c r="H24" s="5">
         <v>21699.96</v>
       </c>
+      <c r="I24" s="5">
+        <f t="shared" ref="I24:I51" si="133">P24*0.5</f>
+        <v>10849.98</v>
+      </c>
+      <c r="J24" s="5">
+        <f t="shared" ref="J24" si="134">I24*0.3</f>
+        <v>3254.9939999999997</v>
+      </c>
+      <c r="K24" s="5">
+        <f t="shared" ref="K24:K51" si="135">I24*1.2</f>
+        <v>13019.975999999999</v>
+      </c>
+      <c r="L24" s="5">
+        <f t="shared" ref="L24:L51" si="136">I24*1.5</f>
+        <v>16274.97</v>
+      </c>
+      <c r="M24" s="5">
+        <f t="shared" ref="M24:M51" si="137">I24*1.9</f>
+        <v>20614.962</v>
+      </c>
+      <c r="N24" s="5">
+        <f t="shared" ref="N24:N51" si="138">I24*0.2</f>
+        <v>2169.9960000000001</v>
+      </c>
+      <c r="O24" s="5">
+        <f t="shared" ref="O24:O51" si="139">I24*1.3</f>
+        <v>14104.974</v>
+      </c>
       <c r="P24" s="5">
         <v>21699.96</v>
       </c>
@@ -1643,14 +2274,14 @@
       <c r="R24" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="S24" s="10">
+      <c r="S24" s="8">
         <v>42251</v>
       </c>
       <c r="T24" s="1" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="25" spans="1:20" ht="12" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:20" ht="13" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>121</v>
       </c>
@@ -1670,9 +2301,34 @@
       <c r="H25" s="5">
         <v>7355.44</v>
       </c>
-      <c r="M25" s="7"/>
-      <c r="N25" s="7"/>
-      <c r="O25" s="7"/>
+      <c r="I25" s="5">
+        <f t="shared" ref="I25:I51" si="140">P25</f>
+        <v>7355.44</v>
+      </c>
+      <c r="J25" s="5">
+        <f t="shared" ref="J25" si="141">I25*0</f>
+        <v>0</v>
+      </c>
+      <c r="K25" s="5">
+        <f t="shared" ref="K25:K51" si="142">I25*1.3</f>
+        <v>9562.0720000000001</v>
+      </c>
+      <c r="L25" s="5">
+        <f t="shared" ref="L25:L51" si="143">I25*1.6</f>
+        <v>11768.704</v>
+      </c>
+      <c r="M25" s="5">
+        <f t="shared" ref="M25:M51" si="144">I25*0.2</f>
+        <v>1471.088</v>
+      </c>
+      <c r="N25" s="5">
+        <f t="shared" ref="N25:N51" si="145">I25*0.5</f>
+        <v>3677.72</v>
+      </c>
+      <c r="O25" s="5">
+        <f t="shared" ref="O25:O51" si="146">I25*1.76</f>
+        <v>12945.5744</v>
+      </c>
       <c r="P25" s="5">
         <v>7355.44</v>
       </c>
@@ -1682,14 +2338,14 @@
       <c r="R25" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="S25" s="10">
+      <c r="S25" s="8">
         <v>42851</v>
       </c>
       <c r="T25" s="1" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="26" spans="1:20" ht="12" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:20" ht="13" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>121</v>
       </c>
@@ -1708,6 +2364,34 @@
       <c r="H26" s="5">
         <v>5030.6400000000003</v>
       </c>
+      <c r="I26" s="5">
+        <f t="shared" ref="I26:I51" si="147">P26*2</f>
+        <v>10061.280000000001</v>
+      </c>
+      <c r="J26" s="5">
+        <f t="shared" ref="J26" si="148">I26*0.8</f>
+        <v>8049.0240000000013</v>
+      </c>
+      <c r="K26" s="5">
+        <f t="shared" ref="K26:K51" si="149">I26*1.1</f>
+        <v>11067.408000000001</v>
+      </c>
+      <c r="L26" s="5">
+        <f t="shared" ref="L26:L51" si="150">I26*1.4</f>
+        <v>14085.791999999999</v>
+      </c>
+      <c r="M26" s="5">
+        <f t="shared" ref="M26:M51" si="151">I26*1.7</f>
+        <v>17104.175999999999</v>
+      </c>
+      <c r="N26" s="5">
+        <f t="shared" ref="N26:N51" si="152">I26*0.1</f>
+        <v>1006.1280000000002</v>
+      </c>
+      <c r="O26" s="5">
+        <f t="shared" ref="O26:O51" si="153">I26*0.05</f>
+        <v>503.06400000000008</v>
+      </c>
       <c r="P26" s="5">
         <v>5030.6400000000003</v>
       </c>
@@ -1721,7 +2405,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="27" spans="1:20" ht="12" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:20" ht="13" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>121</v>
       </c>
@@ -1737,8 +2421,40 @@
       <c r="F27" s="1">
         <v>30</v>
       </c>
-      <c r="I27" s="6"/>
-      <c r="P27" s="5"/>
+      <c r="H27" s="5">
+        <v>0</v>
+      </c>
+      <c r="I27" s="5">
+        <f t="shared" ref="I27:I51" si="154">P27*0.5</f>
+        <v>0</v>
+      </c>
+      <c r="J27" s="5">
+        <f t="shared" ref="J27" si="155">I27*0.3</f>
+        <v>0</v>
+      </c>
+      <c r="K27" s="5">
+        <f t="shared" ref="K27:K51" si="156">I27*1.2</f>
+        <v>0</v>
+      </c>
+      <c r="L27" s="5">
+        <f t="shared" ref="L27:L51" si="157">I27*1.5</f>
+        <v>0</v>
+      </c>
+      <c r="M27" s="5">
+        <f t="shared" ref="M27:M51" si="158">I27*1.9</f>
+        <v>0</v>
+      </c>
+      <c r="N27" s="5">
+        <f t="shared" ref="N27:N51" si="159">I27*0.2</f>
+        <v>0</v>
+      </c>
+      <c r="O27" s="5">
+        <f t="shared" ref="O27:O51" si="160">I27*1.3</f>
+        <v>0</v>
+      </c>
+      <c r="P27" s="5">
+        <v>0</v>
+      </c>
       <c r="Q27" s="1" t="s">
         <v>96</v>
       </c>
@@ -1749,7 +2465,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="28" spans="1:20" ht="12" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:20" ht="13" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>121</v>
       </c>
@@ -1768,6 +2484,34 @@
       <c r="H28" s="5">
         <v>6325</v>
       </c>
+      <c r="I28" s="5">
+        <f t="shared" ref="I28:I51" si="161">P28</f>
+        <v>6325</v>
+      </c>
+      <c r="J28" s="5">
+        <f t="shared" ref="J28" si="162">I28*0</f>
+        <v>0</v>
+      </c>
+      <c r="K28" s="5">
+        <f t="shared" ref="K28:K51" si="163">I28*1.3</f>
+        <v>8222.5</v>
+      </c>
+      <c r="L28" s="5">
+        <f t="shared" ref="L28:L51" si="164">I28*1.6</f>
+        <v>10120</v>
+      </c>
+      <c r="M28" s="5">
+        <f t="shared" ref="M28:M51" si="165">I28*0.2</f>
+        <v>1265</v>
+      </c>
+      <c r="N28" s="5">
+        <f t="shared" ref="N28:N51" si="166">I28*0.5</f>
+        <v>3162.5</v>
+      </c>
+      <c r="O28" s="5">
+        <f t="shared" ref="O28:O51" si="167">I28*1.76</f>
+        <v>11132</v>
+      </c>
       <c r="P28" s="5">
         <v>6325</v>
       </c>
@@ -1777,14 +2521,14 @@
       <c r="R28" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="S28" s="10">
+      <c r="S28" s="8">
         <v>43752</v>
       </c>
       <c r="T28" s="1" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="29" spans="1:20" ht="12" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:20" ht="13" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>121</v>
       </c>
@@ -1803,7 +2547,34 @@
       <c r="H29" s="5">
         <v>24150</v>
       </c>
-      <c r="I29" s="6"/>
+      <c r="I29" s="5">
+        <f t="shared" ref="I29:I51" si="168">P29*2</f>
+        <v>48300</v>
+      </c>
+      <c r="J29" s="5">
+        <f t="shared" ref="J29" si="169">I29*0.8</f>
+        <v>38640</v>
+      </c>
+      <c r="K29" s="5">
+        <f t="shared" ref="K29:K51" si="170">I29*1.1</f>
+        <v>53130.000000000007</v>
+      </c>
+      <c r="L29" s="5">
+        <f t="shared" ref="L29:L51" si="171">I29*1.4</f>
+        <v>67620</v>
+      </c>
+      <c r="M29" s="5">
+        <f t="shared" ref="M29:M51" si="172">I29*1.7</f>
+        <v>82110</v>
+      </c>
+      <c r="N29" s="5">
+        <f t="shared" ref="N29:N51" si="173">I29*0.1</f>
+        <v>4830</v>
+      </c>
+      <c r="O29" s="5">
+        <f t="shared" ref="O29:O51" si="174">I29*0.05</f>
+        <v>2415</v>
+      </c>
       <c r="P29" s="5">
         <v>24150</v>
       </c>
@@ -1817,7 +2588,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="30" spans="1:20" ht="12" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:20" ht="13" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>121</v>
       </c>
@@ -1836,9 +2607,34 @@
       <c r="H30" s="5">
         <v>37986.800000000003</v>
       </c>
-      <c r="M30" s="7"/>
-      <c r="N30" s="7"/>
-      <c r="O30" s="7"/>
+      <c r="I30" s="5">
+        <f t="shared" ref="I30:I51" si="175">P30*0.5</f>
+        <v>18993.400000000001</v>
+      </c>
+      <c r="J30" s="5">
+        <f t="shared" ref="J30" si="176">I30*0.3</f>
+        <v>5698.02</v>
+      </c>
+      <c r="K30" s="5">
+        <f t="shared" ref="K30:K51" si="177">I30*1.2</f>
+        <v>22792.080000000002</v>
+      </c>
+      <c r="L30" s="5">
+        <f t="shared" ref="L30:L51" si="178">I30*1.5</f>
+        <v>28490.100000000002</v>
+      </c>
+      <c r="M30" s="5">
+        <f t="shared" ref="M30:M51" si="179">I30*1.9</f>
+        <v>36087.46</v>
+      </c>
+      <c r="N30" s="5">
+        <f t="shared" ref="N30:N51" si="180">I30*0.2</f>
+        <v>3798.6800000000003</v>
+      </c>
+      <c r="O30" s="5">
+        <f t="shared" ref="O30:O51" si="181">I30*1.3</f>
+        <v>24691.420000000002</v>
+      </c>
       <c r="P30" s="5">
         <v>37986.800000000003</v>
       </c>
@@ -1848,14 +2644,14 @@
       <c r="R30" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="S30" s="10">
+      <c r="S30" s="8">
         <v>42844</v>
       </c>
       <c r="T30" s="1" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="31" spans="1:20" ht="12" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:20" ht="13" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
         <v>121</v>
       </c>
@@ -1874,6 +2670,34 @@
       <c r="H31" s="5">
         <v>6963.41</v>
       </c>
+      <c r="I31" s="5">
+        <f t="shared" ref="I31:I51" si="182">P31</f>
+        <v>6963.41</v>
+      </c>
+      <c r="J31" s="5">
+        <f t="shared" ref="J31" si="183">I31*0</f>
+        <v>0</v>
+      </c>
+      <c r="K31" s="5">
+        <f t="shared" ref="K31:K51" si="184">I31*1.3</f>
+        <v>9052.4330000000009</v>
+      </c>
+      <c r="L31" s="5">
+        <f t="shared" ref="L31:L51" si="185">I31*1.6</f>
+        <v>11141.456</v>
+      </c>
+      <c r="M31" s="5">
+        <f t="shared" ref="M31:M51" si="186">I31*0.2</f>
+        <v>1392.682</v>
+      </c>
+      <c r="N31" s="5">
+        <f t="shared" ref="N31:N51" si="187">I31*0.5</f>
+        <v>3481.7049999999999</v>
+      </c>
+      <c r="O31" s="5">
+        <f t="shared" ref="O31:O51" si="188">I31*1.76</f>
+        <v>12255.6016</v>
+      </c>
       <c r="P31" s="5">
         <v>6963.41</v>
       </c>
@@ -1887,7 +2711,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="32" spans="1:20" ht="12" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:20" ht="13" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
         <v>121</v>
       </c>
@@ -1906,6 +2730,34 @@
       <c r="H32" s="5">
         <v>6863.01</v>
       </c>
+      <c r="I32" s="5">
+        <f t="shared" ref="I32:I51" si="189">P32*2</f>
+        <v>13726.02</v>
+      </c>
+      <c r="J32" s="5">
+        <f t="shared" ref="J32" si="190">I32*0.8</f>
+        <v>10980.816000000001</v>
+      </c>
+      <c r="K32" s="5">
+        <f t="shared" ref="K32:K51" si="191">I32*1.1</f>
+        <v>15098.622000000001</v>
+      </c>
+      <c r="L32" s="5">
+        <f t="shared" ref="L32:L51" si="192">I32*1.4</f>
+        <v>19216.428</v>
+      </c>
+      <c r="M32" s="5">
+        <f t="shared" ref="M32:M51" si="193">I32*1.7</f>
+        <v>23334.234</v>
+      </c>
+      <c r="N32" s="5">
+        <f t="shared" ref="N32:N51" si="194">I32*0.1</f>
+        <v>1372.6020000000001</v>
+      </c>
+      <c r="O32" s="5">
+        <f t="shared" ref="O32:O51" si="195">I32*0.05</f>
+        <v>686.30100000000004</v>
+      </c>
       <c r="P32" s="5">
         <v>6863.01</v>
       </c>
@@ -1919,7 +2771,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="33" spans="1:20" ht="12" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:20" ht="13" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
         <v>121</v>
       </c>
@@ -1935,7 +2787,40 @@
       <c r="F33" s="1">
         <v>30</v>
       </c>
-      <c r="P33" s="5"/>
+      <c r="H33" s="5">
+        <v>0</v>
+      </c>
+      <c r="I33" s="5">
+        <f t="shared" ref="I33:I51" si="196">P33*0.5</f>
+        <v>0</v>
+      </c>
+      <c r="J33" s="5">
+        <f t="shared" ref="J33" si="197">I33*0.3</f>
+        <v>0</v>
+      </c>
+      <c r="K33" s="5">
+        <f t="shared" ref="K33:K51" si="198">I33*1.2</f>
+        <v>0</v>
+      </c>
+      <c r="L33" s="5">
+        <f t="shared" ref="L33:L51" si="199">I33*1.5</f>
+        <v>0</v>
+      </c>
+      <c r="M33" s="5">
+        <f t="shared" ref="M33:M51" si="200">I33*1.9</f>
+        <v>0</v>
+      </c>
+      <c r="N33" s="5">
+        <f t="shared" ref="N33:N51" si="201">I33*0.2</f>
+        <v>0</v>
+      </c>
+      <c r="O33" s="5">
+        <f t="shared" ref="O33:O51" si="202">I33*1.3</f>
+        <v>0</v>
+      </c>
+      <c r="P33" s="5">
+        <v>0</v>
+      </c>
       <c r="Q33" s="1" t="s">
         <v>96</v>
       </c>
@@ -1946,7 +2831,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="34" spans="1:20" ht="12" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:20" ht="13" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
         <v>121</v>
       </c>
@@ -1965,7 +2850,34 @@
       <c r="H34" s="5">
         <v>6367.36</v>
       </c>
-      <c r="I34" s="6"/>
+      <c r="I34" s="5">
+        <f t="shared" ref="I34:I51" si="203">P34</f>
+        <v>6367.36</v>
+      </c>
+      <c r="J34" s="5">
+        <f t="shared" ref="J34" si="204">I34*0</f>
+        <v>0</v>
+      </c>
+      <c r="K34" s="5">
+        <f t="shared" ref="K34:K51" si="205">I34*1.3</f>
+        <v>8277.5679999999993</v>
+      </c>
+      <c r="L34" s="5">
+        <f t="shared" ref="L34:L51" si="206">I34*1.6</f>
+        <v>10187.776</v>
+      </c>
+      <c r="M34" s="5">
+        <f t="shared" ref="M34:M51" si="207">I34*0.2</f>
+        <v>1273.472</v>
+      </c>
+      <c r="N34" s="5">
+        <f t="shared" ref="N34:N51" si="208">I34*0.5</f>
+        <v>3183.68</v>
+      </c>
+      <c r="O34" s="5">
+        <f t="shared" ref="O34:O51" si="209">I34*1.76</f>
+        <v>11206.553599999999</v>
+      </c>
       <c r="P34" s="5">
         <v>6367.36</v>
       </c>
@@ -1975,14 +2887,14 @@
       <c r="R34" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="S34" s="10">
+      <c r="S34" s="8">
         <v>42857</v>
       </c>
       <c r="T34" s="1" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="35" spans="1:20" ht="12" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:20" ht="13" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
         <v>121</v>
       </c>
@@ -2001,9 +2913,34 @@
       <c r="H35" s="5">
         <v>5116.7</v>
       </c>
-      <c r="M35" s="7"/>
-      <c r="N35" s="7"/>
-      <c r="O35" s="7"/>
+      <c r="I35" s="5">
+        <f t="shared" ref="I35:I51" si="210">P35*2</f>
+        <v>10233.4</v>
+      </c>
+      <c r="J35" s="5">
+        <f t="shared" ref="J35" si="211">I35*0.8</f>
+        <v>8186.72</v>
+      </c>
+      <c r="K35" s="5">
+        <f t="shared" ref="K35:K51" si="212">I35*1.1</f>
+        <v>11256.74</v>
+      </c>
+      <c r="L35" s="5">
+        <f t="shared" ref="L35:L51" si="213">I35*1.4</f>
+        <v>14326.759999999998</v>
+      </c>
+      <c r="M35" s="5">
+        <f t="shared" ref="M35:M51" si="214">I35*1.7</f>
+        <v>17396.78</v>
+      </c>
+      <c r="N35" s="5">
+        <f t="shared" ref="N35:N51" si="215">I35*0.1</f>
+        <v>1023.34</v>
+      </c>
+      <c r="O35" s="5">
+        <f t="shared" ref="O35:O51" si="216">I35*0.05</f>
+        <v>511.67</v>
+      </c>
       <c r="P35" s="5">
         <v>5116.7</v>
       </c>
@@ -2013,14 +2950,14 @@
       <c r="R35" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="S35" s="10">
+      <c r="S35" s="8">
         <v>43447</v>
       </c>
       <c r="T35" s="1" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="36" spans="1:20" ht="12" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:20" ht="13" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
         <v>121</v>
       </c>
@@ -2039,6 +2976,34 @@
       <c r="H36" s="5">
         <v>4743.3100000000004</v>
       </c>
+      <c r="I36" s="5">
+        <f t="shared" ref="I36:I51" si="217">P36*0.5</f>
+        <v>2371.6550000000002</v>
+      </c>
+      <c r="J36" s="5">
+        <f t="shared" ref="J36" si="218">I36*0.3</f>
+        <v>711.49650000000008</v>
+      </c>
+      <c r="K36" s="5">
+        <f t="shared" ref="K36:K51" si="219">I36*1.2</f>
+        <v>2845.9860000000003</v>
+      </c>
+      <c r="L36" s="5">
+        <f t="shared" ref="L36:L51" si="220">I36*1.5</f>
+        <v>3557.4825000000001</v>
+      </c>
+      <c r="M36" s="5">
+        <f t="shared" ref="M36:M51" si="221">I36*1.9</f>
+        <v>4506.1445000000003</v>
+      </c>
+      <c r="N36" s="5">
+        <f t="shared" ref="N36:N51" si="222">I36*0.2</f>
+        <v>474.33100000000007</v>
+      </c>
+      <c r="O36" s="5">
+        <f t="shared" ref="O36:O51" si="223">I36*1.3</f>
+        <v>3083.1515000000004</v>
+      </c>
       <c r="P36" s="5">
         <v>4743.3100000000004</v>
       </c>
@@ -2048,14 +3013,14 @@
       <c r="R36" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="S36" s="10">
+      <c r="S36" s="8">
         <v>43383</v>
       </c>
       <c r="T36" s="1" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="37" spans="1:20" ht="12" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:20" ht="13" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
         <v>121</v>
       </c>
@@ -2074,6 +3039,34 @@
       <c r="H37" s="5">
         <v>193540.4</v>
       </c>
+      <c r="I37" s="5">
+        <f t="shared" ref="I37:I51" si="224">P37</f>
+        <v>193540.4</v>
+      </c>
+      <c r="J37" s="5">
+        <f t="shared" ref="J37" si="225">I37*0</f>
+        <v>0</v>
+      </c>
+      <c r="K37" s="5">
+        <f t="shared" ref="K37:K51" si="226">I37*1.3</f>
+        <v>251602.52</v>
+      </c>
+      <c r="L37" s="5">
+        <f t="shared" ref="L37:L51" si="227">I37*1.6</f>
+        <v>309664.64000000001</v>
+      </c>
+      <c r="M37" s="5">
+        <f t="shared" ref="M37:M51" si="228">I37*0.2</f>
+        <v>38708.080000000002</v>
+      </c>
+      <c r="N37" s="5">
+        <f t="shared" ref="N37:N51" si="229">I37*0.5</f>
+        <v>96770.2</v>
+      </c>
+      <c r="O37" s="5">
+        <f t="shared" ref="O37:O51" si="230">I37*1.76</f>
+        <v>340631.10399999999</v>
+      </c>
       <c r="P37" s="5">
         <v>193540.4</v>
       </c>
@@ -2087,7 +3080,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="38" spans="1:20" ht="12" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:20" ht="13" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
         <v>121</v>
       </c>
@@ -2107,6 +3100,34 @@
       <c r="H38" s="5">
         <v>6325</v>
       </c>
+      <c r="I38" s="5">
+        <f t="shared" ref="I38:I51" si="231">P38*2</f>
+        <v>12650</v>
+      </c>
+      <c r="J38" s="5">
+        <f t="shared" ref="J38" si="232">I38*0.8</f>
+        <v>10120</v>
+      </c>
+      <c r="K38" s="5">
+        <f t="shared" ref="K38:K51" si="233">I38*1.1</f>
+        <v>13915.000000000002</v>
+      </c>
+      <c r="L38" s="5">
+        <f t="shared" ref="L38:L51" si="234">I38*1.4</f>
+        <v>17710</v>
+      </c>
+      <c r="M38" s="5">
+        <f t="shared" ref="M38:M51" si="235">I38*1.7</f>
+        <v>21505</v>
+      </c>
+      <c r="N38" s="5">
+        <f t="shared" ref="N38:N51" si="236">I38*0.1</f>
+        <v>1265</v>
+      </c>
+      <c r="O38" s="5">
+        <f t="shared" ref="O38:O51" si="237">I38*0.05</f>
+        <v>632.5</v>
+      </c>
       <c r="P38" s="5">
         <v>6325</v>
       </c>
@@ -2120,7 +3141,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="39" spans="1:20" ht="12" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:20" ht="13" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
         <v>121</v>
       </c>
@@ -2137,6 +3158,34 @@
       <c r="H39" s="5">
         <v>30395.82</v>
       </c>
+      <c r="I39" s="5">
+        <f t="shared" ref="I39:I51" si="238">P39*0.5</f>
+        <v>15197.91</v>
+      </c>
+      <c r="J39" s="5">
+        <f t="shared" ref="J39" si="239">I39*0.3</f>
+        <v>4559.3729999999996</v>
+      </c>
+      <c r="K39" s="5">
+        <f t="shared" ref="K39:K51" si="240">I39*1.2</f>
+        <v>18237.491999999998</v>
+      </c>
+      <c r="L39" s="5">
+        <f t="shared" ref="L39:L51" si="241">I39*1.5</f>
+        <v>22796.864999999998</v>
+      </c>
+      <c r="M39" s="5">
+        <f t="shared" ref="M39:M51" si="242">I39*1.9</f>
+        <v>28876.028999999999</v>
+      </c>
+      <c r="N39" s="5">
+        <f t="shared" ref="N39:N51" si="243">I39*0.2</f>
+        <v>3039.5820000000003</v>
+      </c>
+      <c r="O39" s="5">
+        <f t="shared" ref="O39:O51" si="244">I39*1.3</f>
+        <v>19757.282999999999</v>
+      </c>
       <c r="P39" s="5">
         <v>30395.82</v>
       </c>
@@ -2147,7 +3196,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="40" spans="1:20" ht="12" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:20" ht="13" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
         <v>121</v>
       </c>
@@ -2163,7 +3212,40 @@
       <c r="F40" s="1">
         <v>7</v>
       </c>
-      <c r="P40" s="5"/>
+      <c r="H40" s="5">
+        <v>0</v>
+      </c>
+      <c r="I40" s="5">
+        <f t="shared" ref="I40:I51" si="245">P40</f>
+        <v>0</v>
+      </c>
+      <c r="J40" s="5">
+        <f t="shared" ref="J40" si="246">I40*0</f>
+        <v>0</v>
+      </c>
+      <c r="K40" s="5">
+        <f t="shared" ref="K40:K51" si="247">I40*1.3</f>
+        <v>0</v>
+      </c>
+      <c r="L40" s="5">
+        <f t="shared" ref="L40:L51" si="248">I40*1.6</f>
+        <v>0</v>
+      </c>
+      <c r="M40" s="5">
+        <f t="shared" ref="M40:M51" si="249">I40*0.2</f>
+        <v>0</v>
+      </c>
+      <c r="N40" s="5">
+        <f t="shared" ref="N40:N51" si="250">I40*0.5</f>
+        <v>0</v>
+      </c>
+      <c r="O40" s="5">
+        <f t="shared" ref="O40:O51" si="251">I40*1.76</f>
+        <v>0</v>
+      </c>
+      <c r="P40" s="5">
+        <v>0</v>
+      </c>
       <c r="Q40" s="1" t="s">
         <v>98</v>
       </c>
@@ -2174,7 +3256,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="41" spans="1:20" ht="12" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:20" ht="13" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
         <v>121</v>
       </c>
@@ -2193,6 +3275,34 @@
       <c r="H41" s="5">
         <v>8301.2099999999991</v>
       </c>
+      <c r="I41" s="5">
+        <f t="shared" ref="I41:I51" si="252">P41*2</f>
+        <v>16602.419999999998</v>
+      </c>
+      <c r="J41" s="5">
+        <f t="shared" ref="J41" si="253">I41*0.8</f>
+        <v>13281.936</v>
+      </c>
+      <c r="K41" s="5">
+        <f t="shared" ref="K41:K51" si="254">I41*1.1</f>
+        <v>18262.662</v>
+      </c>
+      <c r="L41" s="5">
+        <f t="shared" ref="L41:L51" si="255">I41*1.4</f>
+        <v>23243.387999999995</v>
+      </c>
+      <c r="M41" s="5">
+        <f t="shared" ref="M41:M51" si="256">I41*1.7</f>
+        <v>28224.113999999998</v>
+      </c>
+      <c r="N41" s="5">
+        <f t="shared" ref="N41:N51" si="257">I41*0.1</f>
+        <v>1660.242</v>
+      </c>
+      <c r="O41" s="5">
+        <f t="shared" ref="O41:O51" si="258">I41*0.05</f>
+        <v>830.12099999999998</v>
+      </c>
       <c r="P41" s="5">
         <v>8301.2099999999991</v>
       </c>
@@ -2206,7 +3316,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="42" spans="1:20" ht="12" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:20" ht="13" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
         <v>121</v>
       </c>
@@ -2225,6 +3335,34 @@
       <c r="H42" s="5">
         <v>40919.9</v>
       </c>
+      <c r="I42" s="5">
+        <f t="shared" ref="I42:I51" si="259">P42*0.5</f>
+        <v>20459.95</v>
+      </c>
+      <c r="J42" s="5">
+        <f t="shared" ref="J42" si="260">I42*0.3</f>
+        <v>6137.9849999999997</v>
+      </c>
+      <c r="K42" s="5">
+        <f t="shared" ref="K42:K51" si="261">I42*1.2</f>
+        <v>24551.94</v>
+      </c>
+      <c r="L42" s="5">
+        <f t="shared" ref="L42:L51" si="262">I42*1.5</f>
+        <v>30689.925000000003</v>
+      </c>
+      <c r="M42" s="5">
+        <f t="shared" ref="M42:M51" si="263">I42*1.9</f>
+        <v>38873.904999999999</v>
+      </c>
+      <c r="N42" s="5">
+        <f t="shared" ref="N42:N51" si="264">I42*0.2</f>
+        <v>4091.9900000000002</v>
+      </c>
+      <c r="O42" s="5">
+        <f t="shared" ref="O42:O51" si="265">I42*1.3</f>
+        <v>26597.935000000001</v>
+      </c>
       <c r="P42" s="5">
         <v>40919.9</v>
       </c>
@@ -2238,7 +3376,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="43" spans="1:20" ht="12" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:20" ht="13" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
         <v>121</v>
       </c>
@@ -2254,21 +3392,54 @@
       <c r="F43" s="1">
         <v>30</v>
       </c>
-      <c r="P43" s="5"/>
+      <c r="H43" s="5">
+        <v>0</v>
+      </c>
+      <c r="I43" s="5">
+        <f t="shared" ref="I43:I51" si="266">P43</f>
+        <v>0</v>
+      </c>
+      <c r="J43" s="5">
+        <f t="shared" ref="J43" si="267">I43*0</f>
+        <v>0</v>
+      </c>
+      <c r="K43" s="5">
+        <f t="shared" ref="K43:K51" si="268">I43*1.3</f>
+        <v>0</v>
+      </c>
+      <c r="L43" s="5">
+        <f t="shared" ref="L43:L51" si="269">I43*1.6</f>
+        <v>0</v>
+      </c>
+      <c r="M43" s="5">
+        <f t="shared" ref="M43:M51" si="270">I43*0.2</f>
+        <v>0</v>
+      </c>
+      <c r="N43" s="5">
+        <f t="shared" ref="N43:N51" si="271">I43*0.5</f>
+        <v>0</v>
+      </c>
+      <c r="O43" s="5">
+        <f t="shared" ref="O43:O51" si="272">I43*1.76</f>
+        <v>0</v>
+      </c>
+      <c r="P43" s="5">
+        <v>0</v>
+      </c>
       <c r="Q43" s="1" t="s">
         <v>96</v>
       </c>
       <c r="R43" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="S43" s="10">
+      <c r="S43" s="8">
         <v>43080</v>
       </c>
       <c r="T43" s="1" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="44" spans="1:20" ht="12" x14ac:dyDescent="0.15">
+    <row r="44" spans="1:20" ht="13" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
         <v>121</v>
       </c>
@@ -2287,6 +3458,34 @@
       <c r="H44" s="5">
         <v>7116</v>
       </c>
+      <c r="I44" s="5">
+        <f t="shared" ref="I44:I51" si="273">P44*2</f>
+        <v>14232</v>
+      </c>
+      <c r="J44" s="5">
+        <f t="shared" ref="J44" si="274">I44*0.8</f>
+        <v>11385.6</v>
+      </c>
+      <c r="K44" s="5">
+        <f t="shared" ref="K44:K51" si="275">I44*1.1</f>
+        <v>15655.2</v>
+      </c>
+      <c r="L44" s="5">
+        <f t="shared" ref="L44:L51" si="276">I44*1.4</f>
+        <v>19924.8</v>
+      </c>
+      <c r="M44" s="5">
+        <f t="shared" ref="M44:M51" si="277">I44*1.7</f>
+        <v>24194.399999999998</v>
+      </c>
+      <c r="N44" s="5">
+        <f t="shared" ref="N44:N51" si="278">I44*0.1</f>
+        <v>1423.2</v>
+      </c>
+      <c r="O44" s="5">
+        <f t="shared" ref="O44:O51" si="279">I44*0.05</f>
+        <v>711.6</v>
+      </c>
       <c r="P44" s="5">
         <v>7116</v>
       </c>
@@ -2296,14 +3495,14 @@
       <c r="R44" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="S44" s="10">
+      <c r="S44" s="8">
         <v>42877</v>
       </c>
       <c r="T44" s="3" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="45" spans="1:20" ht="12" x14ac:dyDescent="0.15">
+    <row r="45" spans="1:20" ht="13" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
         <v>121</v>
       </c>
@@ -2322,6 +3521,34 @@
       <c r="H45" s="5">
         <v>6469.35</v>
       </c>
+      <c r="I45" s="5">
+        <f t="shared" ref="I45:I51" si="280">P45*0.5</f>
+        <v>3234.6750000000002</v>
+      </c>
+      <c r="J45" s="5">
+        <f t="shared" ref="J45" si="281">I45*0.3</f>
+        <v>970.40250000000003</v>
+      </c>
+      <c r="K45" s="5">
+        <f t="shared" ref="K45:K51" si="282">I45*1.2</f>
+        <v>3881.61</v>
+      </c>
+      <c r="L45" s="5">
+        <f t="shared" ref="L45:L51" si="283">I45*1.5</f>
+        <v>4852.0125000000007</v>
+      </c>
+      <c r="M45" s="5">
+        <f t="shared" ref="M45:M51" si="284">I45*1.9</f>
+        <v>6145.8824999999997</v>
+      </c>
+      <c r="N45" s="5">
+        <f t="shared" ref="N45:N51" si="285">I45*0.2</f>
+        <v>646.93500000000006</v>
+      </c>
+      <c r="O45" s="5">
+        <f t="shared" ref="O45:O51" si="286">I45*1.3</f>
+        <v>4205.0775000000003</v>
+      </c>
       <c r="P45" s="5">
         <v>6469.35</v>
       </c>
@@ -2335,7 +3562,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="46" spans="1:20" ht="12" x14ac:dyDescent="0.15">
+    <row r="46" spans="1:20" ht="13" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
         <v>121</v>
       </c>
@@ -2355,6 +3582,34 @@
       <c r="H46" s="5">
         <v>5227.2</v>
       </c>
+      <c r="I46" s="5">
+        <f t="shared" ref="I46:I51" si="287">P46</f>
+        <v>5227.2</v>
+      </c>
+      <c r="J46" s="5">
+        <f t="shared" ref="J46" si="288">I46*0</f>
+        <v>0</v>
+      </c>
+      <c r="K46" s="5">
+        <f t="shared" ref="K46:K51" si="289">I46*1.3</f>
+        <v>6795.36</v>
+      </c>
+      <c r="L46" s="5">
+        <f t="shared" ref="L46:L51" si="290">I46*1.6</f>
+        <v>8363.52</v>
+      </c>
+      <c r="M46" s="5">
+        <f t="shared" ref="M46:M51" si="291">I46*0.2</f>
+        <v>1045.44</v>
+      </c>
+      <c r="N46" s="5">
+        <f t="shared" ref="N46:N51" si="292">I46*0.5</f>
+        <v>2613.6</v>
+      </c>
+      <c r="O46" s="5">
+        <f t="shared" ref="O46:O51" si="293">I46*1.76</f>
+        <v>9199.8719999999994</v>
+      </c>
       <c r="P46" s="5">
         <v>5227.2</v>
       </c>
@@ -2368,7 +3623,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="47" spans="1:20" ht="12" x14ac:dyDescent="0.15">
+    <row r="47" spans="1:20" ht="13" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
         <v>121</v>
       </c>
@@ -2384,6 +3639,34 @@
       <c r="H47" s="5">
         <v>9348</v>
       </c>
+      <c r="I47" s="5">
+        <f t="shared" ref="I47:I51" si="294">P47*2</f>
+        <v>18696</v>
+      </c>
+      <c r="J47" s="5">
+        <f t="shared" ref="J47" si="295">I47*0.8</f>
+        <v>14956.800000000001</v>
+      </c>
+      <c r="K47" s="5">
+        <f t="shared" ref="K47:K51" si="296">I47*1.1</f>
+        <v>20565.600000000002</v>
+      </c>
+      <c r="L47" s="5">
+        <f t="shared" ref="L47:L51" si="297">I47*1.4</f>
+        <v>26174.399999999998</v>
+      </c>
+      <c r="M47" s="5">
+        <f t="shared" ref="M47:M51" si="298">I47*1.7</f>
+        <v>31783.200000000001</v>
+      </c>
+      <c r="N47" s="5">
+        <f t="shared" ref="N47:N51" si="299">I47*0.1</f>
+        <v>1869.6000000000001</v>
+      </c>
+      <c r="O47" s="5">
+        <f t="shared" ref="O47:O51" si="300">I47*0.05</f>
+        <v>934.80000000000007</v>
+      </c>
       <c r="P47" s="5">
         <v>9348</v>
       </c>
@@ -2391,7 +3674,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="48" spans="1:20" ht="12" x14ac:dyDescent="0.15">
+    <row r="48" spans="1:20" ht="13" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
         <v>121</v>
       </c>
@@ -2411,6 +3694,34 @@
       <c r="H48" s="5">
         <v>8202</v>
       </c>
+      <c r="I48" s="5">
+        <f t="shared" ref="I48:I51" si="301">P48*0.5</f>
+        <v>4101</v>
+      </c>
+      <c r="J48" s="5">
+        <f t="shared" ref="J48" si="302">I48*0.3</f>
+        <v>1230.3</v>
+      </c>
+      <c r="K48" s="5">
+        <f t="shared" ref="K48:K51" si="303">I48*1.2</f>
+        <v>4921.2</v>
+      </c>
+      <c r="L48" s="5">
+        <f t="shared" ref="L48:L51" si="304">I48*1.5</f>
+        <v>6151.5</v>
+      </c>
+      <c r="M48" s="5">
+        <f t="shared" ref="M48:M51" si="305">I48*1.9</f>
+        <v>7791.9</v>
+      </c>
+      <c r="N48" s="5">
+        <f t="shared" ref="N48:N51" si="306">I48*0.2</f>
+        <v>820.2</v>
+      </c>
+      <c r="O48" s="5">
+        <f t="shared" ref="O48:O51" si="307">I48*1.3</f>
+        <v>5331.3</v>
+      </c>
       <c r="P48" s="5">
         <v>8202</v>
       </c>
@@ -2424,7 +3735,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="49" spans="1:20" ht="12" x14ac:dyDescent="0.15">
+    <row r="49" spans="1:20" ht="13" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
         <v>121</v>
       </c>
@@ -2443,6 +3754,34 @@
       <c r="H49" s="5">
         <v>8634.1</v>
       </c>
+      <c r="I49" s="5">
+        <f t="shared" ref="I49:I51" si="308">P49</f>
+        <v>8634.1</v>
+      </c>
+      <c r="J49" s="5">
+        <f t="shared" ref="J49" si="309">I49*0</f>
+        <v>0</v>
+      </c>
+      <c r="K49" s="5">
+        <f t="shared" ref="K49:K51" si="310">I49*1.3</f>
+        <v>11224.330000000002</v>
+      </c>
+      <c r="L49" s="5">
+        <f t="shared" ref="L49:L51" si="311">I49*1.6</f>
+        <v>13814.560000000001</v>
+      </c>
+      <c r="M49" s="5">
+        <f t="shared" ref="M49:M51" si="312">I49*0.2</f>
+        <v>1726.8200000000002</v>
+      </c>
+      <c r="N49" s="5">
+        <f t="shared" ref="N49:N51" si="313">I49*0.5</f>
+        <v>4317.05</v>
+      </c>
+      <c r="O49" s="5">
+        <f t="shared" ref="O49:O51" si="314">I49*1.76</f>
+        <v>15196.016000000001</v>
+      </c>
       <c r="P49" s="5">
         <v>8634.1</v>
       </c>
@@ -2452,14 +3791,14 @@
       <c r="R49" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="S49" s="10">
+      <c r="S49" s="8">
         <v>43071</v>
       </c>
       <c r="T49" s="1" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="50" spans="1:20" ht="12" x14ac:dyDescent="0.15">
+    <row r="50" spans="1:20" ht="13" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
         <v>121</v>
       </c>
@@ -2478,6 +3817,34 @@
       <c r="H50" s="5">
         <v>5131.25</v>
       </c>
+      <c r="I50" s="5">
+        <f t="shared" ref="I50:I51" si="315">P50*2</f>
+        <v>10262.5</v>
+      </c>
+      <c r="J50" s="5">
+        <f t="shared" ref="J50" si="316">I50*0.8</f>
+        <v>8210</v>
+      </c>
+      <c r="K50" s="5">
+        <f t="shared" ref="K50:K51" si="317">I50*1.1</f>
+        <v>11288.750000000002</v>
+      </c>
+      <c r="L50" s="5">
+        <f t="shared" ref="L50:L51" si="318">I50*1.4</f>
+        <v>14367.499999999998</v>
+      </c>
+      <c r="M50" s="5">
+        <f t="shared" ref="M50:M51" si="319">I50*1.7</f>
+        <v>17446.25</v>
+      </c>
+      <c r="N50" s="5">
+        <f t="shared" ref="N50:N51" si="320">I50*0.1</f>
+        <v>1026.25</v>
+      </c>
+      <c r="O50" s="5">
+        <f t="shared" ref="O50:O51" si="321">I50*0.05</f>
+        <v>513.125</v>
+      </c>
       <c r="P50" s="5">
         <v>5131.25</v>
       </c>
@@ -2491,7 +3858,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="51" spans="1:20" ht="12" x14ac:dyDescent="0.15">
+    <row r="51" spans="1:20" ht="13" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
         <v>121</v>
       </c>
@@ -2510,6 +3877,34 @@
       <c r="H51" s="5">
         <v>5495</v>
       </c>
+      <c r="I51" s="5">
+        <f t="shared" ref="I51" si="322">P51*0.5</f>
+        <v>2747.5</v>
+      </c>
+      <c r="J51" s="5">
+        <f t="shared" ref="J51" si="323">I51*0.3</f>
+        <v>824.25</v>
+      </c>
+      <c r="K51" s="5">
+        <f t="shared" ref="K51" si="324">I51*1.2</f>
+        <v>3297</v>
+      </c>
+      <c r="L51" s="5">
+        <f t="shared" ref="L51" si="325">I51*1.5</f>
+        <v>4121.25</v>
+      </c>
+      <c r="M51" s="5">
+        <f t="shared" ref="M51" si="326">I51*1.9</f>
+        <v>5220.25</v>
+      </c>
+      <c r="N51" s="5">
+        <f t="shared" ref="N51" si="327">I51*0.2</f>
+        <v>549.5</v>
+      </c>
+      <c r="O51" s="5">
+        <f t="shared" ref="O51" si="328">I51*1.3</f>
+        <v>3571.75</v>
+      </c>
       <c r="P51" s="5">
         <v>5495</v>
       </c>
@@ -2519,7 +3914,7 @@
       <c r="R51" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="S51" s="10">
+      <c r="S51" s="8">
         <v>43132</v>
       </c>
       <c r="T51" s="1" t="s">

</xml_diff>